<commit_message>
startup not working, but commands hardcoded and comms in place. Using WT V/I from outside switch working so far to allow turbine to come back from short trips
</commit_message>
<xml_diff>
--- a/CART dependencies/Microgrid_cmd.xlsx
+++ b/CART dependencies/Microgrid_cmd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Autonomous-Microgrid-Control-with-Forecasting\CART dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E4E448-FA96-46A3-9EA4-1D28DF6894FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D9DECE-BC1C-4581-B736-BCAD11D80368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
+    <workbookView minimized="1" xWindow="885" yWindow="885" windowWidth="3960" windowHeight="2940" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
   </bookViews>
   <sheets>
     <sheet name="WTGmode" sheetId="13" r:id="rId1"/>
@@ -416,7 +416,7 @@
   <dimension ref="A1:B452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20581,7 +20581,7 @@
       </c>
       <c r="B2">
         <f ca="1">575+0.5*RAND()</f>
-        <v>575.25803337781792</v>
+        <v>575.23117074936567</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -20590,7 +20590,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B52" ca="1" si="0">575+0.5*RAND()</f>
-        <v>575.34339048857521</v>
+        <v>575.27856327094139</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -20599,7 +20599,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>575.0777398276183</v>
+        <v>575.08298487843365</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -20608,7 +20608,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>575.07127925730015</v>
+        <v>575.47162436143594</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -20617,7 +20617,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>575.11136479100651</v>
+        <v>575.42848255203546</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -20626,7 +20626,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>575.09687689032091</v>
+        <v>575.4674224189605</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -20635,7 +20635,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>575.29290157730077</v>
+        <v>575.04252945113717</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -20644,7 +20644,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>575.48180688914965</v>
+        <v>575.07086488076084</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -20653,7 +20653,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>575.14831281913825</v>
+        <v>575.03530769001406</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -20662,7 +20662,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>575.23467725052365</v>
+        <v>575.01483503554778</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -20671,7 +20671,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>575.23629043795711</v>
+        <v>575.47264833575298</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -20680,7 +20680,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>575.05245410710961</v>
+        <v>575.02318929931619</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -20689,7 +20689,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>575.24750956828245</v>
+        <v>575.41153472023075</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -20698,7 +20698,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>575.32102815001588</v>
+        <v>575.47359819706287</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -20707,7 +20707,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>575.43534987234671</v>
+        <v>575.11198842098361</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -20716,7 +20716,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>575.03999658925409</v>
+        <v>575.22877777076189</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -20725,7 +20725,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>575.17310038538892</v>
+        <v>575.46982530541914</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -20734,7 +20734,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>575.13814715846343</v>
+        <v>575.43434524855672</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -20743,7 +20743,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>575.2697135577597</v>
+        <v>575.18413349666491</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -20752,7 +20752,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>575.35059610771373</v>
+        <v>575.30003383393307</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -20761,7 +20761,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>575.2632041547115</v>
+        <v>575.26396620970615</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -20770,7 +20770,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>575.27235049917931</v>
+        <v>575.48531201613355</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -20779,7 +20779,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>575.35245822077593</v>
+        <v>575.3890032748875</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -20788,7 +20788,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>575.24412671150378</v>
+        <v>575.4934564949757</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -20797,7 +20797,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>575.38005208231073</v>
+        <v>575.45312708275151</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -20806,7 +20806,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>575.24093288872393</v>
+        <v>575.45635319522307</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -20815,7 +20815,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>575.02774826678024</v>
+        <v>575.12524617165866</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -20824,7 +20824,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>575.34556866662479</v>
+        <v>575.41846942385132</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -20833,7 +20833,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>575.16705473945342</v>
+        <v>575.26801616049158</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -20842,7 +20842,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>575.48894500968572</v>
+        <v>575.33233341702623</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -20851,7 +20851,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>575.08622996822623</v>
+        <v>575.20184747884036</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -20860,7 +20860,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>575.30702104128443</v>
+        <v>575.38310162286268</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -20869,7 +20869,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>575.19280911998032</v>
+        <v>575.40584199608008</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -20878,7 +20878,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>575.47223598612811</v>
+        <v>575.47843100649027</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -20887,7 +20887,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>575.36446537800998</v>
+        <v>575.03302650035835</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -20896,7 +20896,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>575.45200491246703</v>
+        <v>575.11863214486664</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -20905,7 +20905,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>575.07030088155932</v>
+        <v>575.26377971253987</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -20914,7 +20914,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>575.39961339102479</v>
+        <v>575.09849412719177</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -20923,7 +20923,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>575.31468611555385</v>
+        <v>575.03002175613938</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -20932,7 +20932,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>575.4435105651288</v>
+        <v>575.3041613289513</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -20941,7 +20941,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>575.31019480763007</v>
+        <v>575.26154023721153</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -20950,7 +20950,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>575.13689523738094</v>
+        <v>575.47872187030475</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -20959,7 +20959,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>575.46292058073152</v>
+        <v>575.24715337371379</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -20968,7 +20968,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>575.08917046616375</v>
+        <v>575.17501714053685</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -20977,7 +20977,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="0"/>
-        <v>575.04375313268133</v>
+        <v>575.09697093611635</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -20986,7 +20986,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>575.07995497037984</v>
+        <v>575.39615830739956</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -20995,7 +20995,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>575.4053913451188</v>
+        <v>575.40548048221365</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -21004,7 +21004,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>575.34974971629288</v>
+        <v>575.27411774502264</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -21013,7 +21013,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>575.48639409184273</v>
+        <v>575.01309738770817</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -21022,7 +21022,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>575.47052796410412</v>
+        <v>575.36723294493459</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -21031,7 +21031,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>575.23848974161444</v>
+        <v>575.29095275826796</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -21040,7 +21040,7 @@
       </c>
       <c r="B53">
         <f ca="1">B52-RAND()</f>
-        <v>574.75666448613379</v>
+        <v>574.60806356545083</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -21049,7 +21049,7 @@
       </c>
       <c r="B54">
         <f t="shared" ref="B54:B113" ca="1" si="1">B53-RAND()</f>
-        <v>574.45101809607331</v>
+        <v>573.77903224245154</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -21058,7 +21058,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>573.89340634296332</v>
+        <v>573.46098113569656</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -21067,7 +21067,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>573.25760452042221</v>
+        <v>573.2921594903454</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -21076,7 +21076,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>572.8161405446956</v>
+        <v>573.02225073233421</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -21085,7 +21085,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>572.52242288141315</v>
+        <v>572.37747773911644</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -21094,7 +21094,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>572.30113533546364</v>
+        <v>572.30189449439308</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -21103,7 +21103,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>572.04488445401239</v>
+        <v>571.82048157380632</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -21112,7 +21112,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>571.85370186742523</v>
+        <v>571.66668863624386</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -21121,7 +21121,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>571.62344824052991</v>
+        <v>570.79678389454534</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -21130,7 +21130,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>570.81151077178197</v>
+        <v>570.30941976279667</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -21139,7 +21139,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>569.87324500648697</v>
+        <v>570.26928468679739</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -21148,7 +21148,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>569.07529331541912</v>
+        <v>569.84741379908053</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -21157,7 +21157,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="1"/>
-        <v>568.19749041555258</v>
+        <v>569.62897448739818</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -21166,7 +21166,7 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="1"/>
-        <v>568.02177984300226</v>
+        <v>569.46019084875149</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -21175,7 +21175,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="1"/>
-        <v>567.75200584490005</v>
+        <v>568.58283111974765</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -21184,7 +21184,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="1"/>
-        <v>567.54822682784413</v>
+        <v>568.17755932035493</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -21193,7 +21193,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="1"/>
-        <v>567.41165791615299</v>
+        <v>567.89474736074999</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -21202,7 +21202,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="1"/>
-        <v>566.64714072310255</v>
+        <v>567.50377219618974</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -21211,7 +21211,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="1"/>
-        <v>566.60151153652862</v>
+        <v>567.21104387703065</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -21220,7 +21220,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="1"/>
-        <v>566.54574684838497</v>
+        <v>566.72869171280672</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -21229,7 +21229,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="1"/>
-        <v>565.73104444858075</v>
+        <v>566.45397385049273</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -21238,7 +21238,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="1"/>
-        <v>564.94435158999454</v>
+        <v>565.49144400087914</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -21247,7 +21247,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="1"/>
-        <v>564.38173897810293</v>
+        <v>565.25326560849646</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -21256,7 +21256,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="1"/>
-        <v>564.32277646112107</v>
+        <v>564.29058907234787</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -21265,7 +21265,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="1"/>
-        <v>563.6880680302761</v>
+        <v>564.03813099805814</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -21274,7 +21274,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="1"/>
-        <v>563.09989680574529</v>
+        <v>563.95431079716877</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -21283,7 +21283,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="1"/>
-        <v>562.83326243831152</v>
+        <v>562.97435901733888</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -21292,7 +21292,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="1"/>
-        <v>562.50035505899007</v>
+        <v>562.42725023578282</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -21301,7 +21301,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="1"/>
-        <v>561.60998785098309</v>
+        <v>561.56632996135932</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -21310,7 +21310,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="1"/>
-        <v>561.13719635301413</v>
+        <v>561.15653391269416</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -21319,7 +21319,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="1"/>
-        <v>560.81971447756882</v>
+        <v>560.70541183853356</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -21328,7 +21328,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="1"/>
-        <v>560.32710532076612</v>
+        <v>560.54770190375075</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -21337,7 +21337,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="1"/>
-        <v>559.37384070329256</v>
+        <v>560.26920445006476</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -21346,7 +21346,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="1"/>
-        <v>558.60174491290229</v>
+        <v>559.44385417175886</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -21355,7 +21355,7 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="1"/>
-        <v>558.17296010673988</v>
+        <v>558.48639032705182</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -21364,7 +21364,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="1"/>
-        <v>557.53631478500301</v>
+        <v>557.94166226470907</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -21373,7 +21373,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="1"/>
-        <v>556.7363299780809</v>
+        <v>557.92506452656096</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -21382,7 +21382,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="1"/>
-        <v>556.48317700536506</v>
+        <v>556.9790118156094</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -21391,7 +21391,7 @@
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="1"/>
-        <v>555.64402619111422</v>
+        <v>556.32827467898574</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -21400,7 +21400,7 @@
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="1"/>
-        <v>554.8017904903727</v>
+        <v>556.2577111186165</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -21409,7 +21409,7 @@
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="1"/>
-        <v>554.60432118604467</v>
+        <v>556.12484325742412</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -21418,7 +21418,7 @@
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="1"/>
-        <v>553.99937500773478</v>
+        <v>555.34352137743213</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -21427,7 +21427,7 @@
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="1"/>
-        <v>553.82169456403574</v>
+        <v>554.81386727045356</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -21436,7 +21436,7 @@
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="1"/>
-        <v>553.73034676597695</v>
+        <v>554.31724167098434</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -21445,7 +21445,7 @@
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="1"/>
-        <v>553.66936467616051</v>
+        <v>553.37689570417115</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -21454,7 +21454,7 @@
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="1"/>
-        <v>552.78924543577443</v>
+        <v>553.07177961110733</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -21463,7 +21463,7 @@
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="1"/>
-        <v>551.92345499806027</v>
+        <v>552.61056805793396</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -21472,7 +21472,7 @@
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="1"/>
-        <v>551.55426604821105</v>
+        <v>552.39099510904634</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -21481,7 +21481,7 @@
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="1"/>
-        <v>551.49749873049848</v>
+        <v>552.03369523664105</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -21490,7 +21490,7 @@
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="1"/>
-        <v>550.96484153361882</v>
+        <v>551.378597509869</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -21499,7 +21499,7 @@
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="1"/>
-        <v>550.20827859799249</v>
+        <v>550.8214973565174</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -21508,7 +21508,7 @@
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="1"/>
-        <v>549.90165302971002</v>
+        <v>550.34489461858743</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -21517,7 +21517,7 @@
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="1"/>
-        <v>549.43965368295846</v>
+        <v>549.46441008547129</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -21526,7 +21526,7 @@
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="1"/>
-        <v>549.08025032739374</v>
+        <v>548.99595821809794</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -21535,7 +21535,7 @@
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="1"/>
-        <v>548.51005552685774</v>
+        <v>548.28692140619114</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -21544,7 +21544,7 @@
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="1"/>
-        <v>548.29956192885231</v>
+        <v>548.01178489430367</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -21553,7 +21553,7 @@
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="1"/>
-        <v>547.85670453777777</v>
+        <v>547.95329967442285</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -21562,7 +21562,7 @@
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="1"/>
-        <v>547.02229875903629</v>
+        <v>547.16252102331248</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -21571,7 +21571,7 @@
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="1"/>
-        <v>546.91261053014216</v>
+        <v>546.93818372690635</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -21580,7 +21580,7 @@
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="1"/>
-        <v>546.53773413132262</v>
+        <v>546.13778244175376</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -21589,7 +21589,7 @@
       </c>
       <c r="B114">
         <f ca="1">B113+0.1*RAND()</f>
-        <v>546.57627455169074</v>
+        <v>546.22724080206081</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -21598,7 +21598,7 @@
       </c>
       <c r="B115">
         <f t="shared" ref="B115:B178" ca="1" si="2">B114+0.1*RAND()</f>
-        <v>546.6533524224277</v>
+        <v>546.27829221745822</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -21607,7 +21607,7 @@
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="2"/>
-        <v>546.66091836765349</v>
+        <v>546.32904925628577</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -21616,7 +21616,7 @@
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="2"/>
-        <v>546.69959234492433</v>
+        <v>546.34729546546259</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -21625,7 +21625,7 @@
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="2"/>
-        <v>546.7761770237812</v>
+        <v>546.35771650974436</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -21634,7 +21634,7 @@
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="2"/>
-        <v>546.82049458191602</v>
+        <v>546.37057090419557</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -21643,7 +21643,7 @@
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="2"/>
-        <v>546.85273120397812</v>
+        <v>546.43531668168748</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -21652,7 +21652,7 @@
       </c>
       <c r="B121">
         <f t="shared" ca="1" si="2"/>
-        <v>546.94177680208679</v>
+        <v>546.44471073970215</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -21661,7 +21661,7 @@
       </c>
       <c r="B122">
         <f t="shared" ca="1" si="2"/>
-        <v>547.02178990446635</v>
+        <v>546.50953778740757</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -21670,7 +21670,7 @@
       </c>
       <c r="B123">
         <f t="shared" ca="1" si="2"/>
-        <v>547.06261729707182</v>
+        <v>546.57937483223873</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -21679,7 +21679,7 @@
       </c>
       <c r="B124">
         <f t="shared" ca="1" si="2"/>
-        <v>547.13416365126716</v>
+        <v>546.62517021904659</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -21688,7 +21688,7 @@
       </c>
       <c r="B125">
         <f t="shared" ca="1" si="2"/>
-        <v>547.15549274872762</v>
+        <v>546.63538958059314</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -21697,7 +21697,7 @@
       </c>
       <c r="B126">
         <f t="shared" ca="1" si="2"/>
-        <v>547.22598948341124</v>
+        <v>546.63775605204182</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -21706,7 +21706,7 @@
       </c>
       <c r="B127">
         <f t="shared" ca="1" si="2"/>
-        <v>547.28770763215857</v>
+        <v>546.71932133121447</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -21715,7 +21715,7 @@
       </c>
       <c r="B128">
         <f t="shared" ca="1" si="2"/>
-        <v>547.31821284975467</v>
+        <v>546.74368454762669</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -21724,7 +21724,7 @@
       </c>
       <c r="B129">
         <f t="shared" ca="1" si="2"/>
-        <v>547.34590682224791</v>
+        <v>546.78689629872633</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -21733,7 +21733,7 @@
       </c>
       <c r="B130">
         <f t="shared" ca="1" si="2"/>
-        <v>547.39316452786204</v>
+        <v>546.81726676249355</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -21742,7 +21742,7 @@
       </c>
       <c r="B131">
         <f t="shared" ca="1" si="2"/>
-        <v>547.45065422900836</v>
+        <v>546.89522373116665</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -21751,7 +21751,7 @@
       </c>
       <c r="B132">
         <f t="shared" ca="1" si="2"/>
-        <v>547.52098016434377</v>
+        <v>546.93345874568513</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -21760,7 +21760,7 @@
       </c>
       <c r="B133">
         <f t="shared" ca="1" si="2"/>
-        <v>547.56987937024894</v>
+        <v>546.96530510552543</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -21769,7 +21769,7 @@
       </c>
       <c r="B134">
         <f t="shared" ca="1" si="2"/>
-        <v>547.57264442874452</v>
+        <v>546.99599532909951</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -21778,7 +21778,7 @@
       </c>
       <c r="B135">
         <f t="shared" ca="1" si="2"/>
-        <v>547.58073571699879</v>
+        <v>547.03094230243346</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -21787,7 +21787,7 @@
       </c>
       <c r="B136">
         <f t="shared" ca="1" si="2"/>
-        <v>547.66767549238637</v>
+        <v>547.13060216097927</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -21796,7 +21796,7 @@
       </c>
       <c r="B137">
         <f t="shared" ca="1" si="2"/>
-        <v>547.7577868504253</v>
+        <v>547.13800915443483</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -21805,7 +21805,7 @@
       </c>
       <c r="B138">
         <f t="shared" ca="1" si="2"/>
-        <v>547.80332034794515</v>
+        <v>547.16758027100332</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -21814,7 +21814,7 @@
       </c>
       <c r="B139">
         <f t="shared" ca="1" si="2"/>
-        <v>547.8934809162854</v>
+        <v>547.21269909288435</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -21823,7 +21823,7 @@
       </c>
       <c r="B140">
         <f t="shared" ca="1" si="2"/>
-        <v>547.91252666051912</v>
+        <v>547.29019064376848</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -21832,7 +21832,7 @@
       </c>
       <c r="B141">
         <f t="shared" ca="1" si="2"/>
-        <v>547.97951448719402</v>
+        <v>547.37886443337709</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -21841,7 +21841,7 @@
       </c>
       <c r="B142">
         <f t="shared" ca="1" si="2"/>
-        <v>548.06086734109635</v>
+        <v>547.42085414856206</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -21850,7 +21850,7 @@
       </c>
       <c r="B143">
         <f t="shared" ca="1" si="2"/>
-        <v>548.13911601450536</v>
+        <v>547.4222761743714</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -21859,7 +21859,7 @@
       </c>
       <c r="B144">
         <f t="shared" ca="1" si="2"/>
-        <v>548.2108874156188</v>
+        <v>547.47082064996368</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -21868,7 +21868,7 @@
       </c>
       <c r="B145">
         <f t="shared" ca="1" si="2"/>
-        <v>548.22010879088032</v>
+        <v>547.53689270840732</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -21877,7 +21877,7 @@
       </c>
       <c r="B146">
         <f t="shared" ca="1" si="2"/>
-        <v>548.27320635441129</v>
+        <v>547.60823008534726</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="B147">
         <f t="shared" ca="1" si="2"/>
-        <v>548.29409047483466</v>
+        <v>547.64181529563223</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -21895,7 +21895,7 @@
       </c>
       <c r="B148">
         <f t="shared" ca="1" si="2"/>
-        <v>548.36775582660903</v>
+        <v>547.72130549452027</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -21904,7 +21904,7 @@
       </c>
       <c r="B149">
         <f t="shared" ca="1" si="2"/>
-        <v>548.40280475352688</v>
+        <v>547.77300579326243</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -21913,7 +21913,7 @@
       </c>
       <c r="B150">
         <f t="shared" ca="1" si="2"/>
-        <v>548.41596333080099</v>
+        <v>547.79001653219325</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -21922,7 +21922,7 @@
       </c>
       <c r="B151">
         <f t="shared" ca="1" si="2"/>
-        <v>548.47581518740424</v>
+        <v>547.83484220700211</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -21931,7 +21931,7 @@
       </c>
       <c r="B152">
         <f t="shared" ca="1" si="2"/>
-        <v>548.53938034177395</v>
+        <v>547.93445750258968</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -21940,7 +21940,7 @@
       </c>
       <c r="B153">
         <f t="shared" ca="1" si="2"/>
-        <v>548.55931802661712</v>
+        <v>548.02276709097168</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -21949,7 +21949,7 @@
       </c>
       <c r="B154">
         <f t="shared" ca="1" si="2"/>
-        <v>548.5773087873763</v>
+        <v>548.08616708541649</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -21958,7 +21958,7 @@
       </c>
       <c r="B155">
         <f t="shared" ca="1" si="2"/>
-        <v>548.64218592427198</v>
+        <v>548.10138221125601</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -21967,7 +21967,7 @@
       </c>
       <c r="B156">
         <f t="shared" ca="1" si="2"/>
-        <v>548.68891205962336</v>
+        <v>548.17868594921151</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -21976,7 +21976,7 @@
       </c>
       <c r="B157">
         <f t="shared" ca="1" si="2"/>
-        <v>548.71279765331781</v>
+        <v>548.17891720051466</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -21985,7 +21985,7 @@
       </c>
       <c r="B158">
         <f t="shared" ca="1" si="2"/>
-        <v>548.78050278802345</v>
+        <v>548.23370206571451</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -21994,7 +21994,7 @@
       </c>
       <c r="B159">
         <f t="shared" ca="1" si="2"/>
-        <v>548.87617452760367</v>
+        <v>548.30375560154152</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -22003,7 +22003,7 @@
       </c>
       <c r="B160">
         <f t="shared" ca="1" si="2"/>
-        <v>548.96634054078129</v>
+        <v>548.38828314548562</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -22012,7 +22012,7 @@
       </c>
       <c r="B161">
         <f t="shared" ca="1" si="2"/>
-        <v>549.04024847082439</v>
+        <v>548.43543059974172</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -22021,7 +22021,7 @@
       </c>
       <c r="B162">
         <f t="shared" ca="1" si="2"/>
-        <v>549.13311855232678</v>
+        <v>548.47132439959637</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -22030,7 +22030,7 @@
       </c>
       <c r="B163">
         <f t="shared" ca="1" si="2"/>
-        <v>549.19047108409325</v>
+        <v>548.50458735981158</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -22039,7 +22039,7 @@
       </c>
       <c r="B164">
         <f t="shared" ca="1" si="2"/>
-        <v>549.21390931172061</v>
+        <v>548.58339035552876</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -22048,7 +22048,7 @@
       </c>
       <c r="B165">
         <f t="shared" ca="1" si="2"/>
-        <v>549.29270552565754</v>
+        <v>548.6784838785893</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -22057,7 +22057,7 @@
       </c>
       <c r="B166">
         <f t="shared" ca="1" si="2"/>
-        <v>549.31741667730626</v>
+        <v>548.75326249756711</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -22066,7 +22066,7 @@
       </c>
       <c r="B167">
         <f t="shared" ca="1" si="2"/>
-        <v>549.32996947987283</v>
+        <v>548.77469308902766</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -22075,7 +22075,7 @@
       </c>
       <c r="B168">
         <f t="shared" ca="1" si="2"/>
-        <v>549.34069392892002</v>
+        <v>548.79673047247377</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -22084,7 +22084,7 @@
       </c>
       <c r="B169">
         <f t="shared" ca="1" si="2"/>
-        <v>549.41956952416353</v>
+        <v>548.79737908829907</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -22093,7 +22093,7 @@
       </c>
       <c r="B170">
         <f t="shared" ca="1" si="2"/>
-        <v>549.51373566095879</v>
+        <v>548.83053195296884</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -22102,7 +22102,7 @@
       </c>
       <c r="B171">
         <f t="shared" ca="1" si="2"/>
-        <v>549.5413576762819</v>
+        <v>548.90880933044627</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -22111,7 +22111,7 @@
       </c>
       <c r="B172">
         <f t="shared" ca="1" si="2"/>
-        <v>549.58979943067607</v>
+        <v>548.99323776440895</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -22120,7 +22120,7 @@
       </c>
       <c r="B173">
         <f t="shared" ca="1" si="2"/>
-        <v>549.6019752440435</v>
+        <v>549.03851228188864</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -22129,7 +22129,7 @@
       </c>
       <c r="B174">
         <f t="shared" ca="1" si="2"/>
-        <v>549.64561165731754</v>
+        <v>549.13832252068357</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -22138,7 +22138,7 @@
       </c>
       <c r="B175">
         <f t="shared" ca="1" si="2"/>
-        <v>549.72622025379928</v>
+        <v>549.163156098949</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -22147,7 +22147,7 @@
       </c>
       <c r="B176">
         <f t="shared" ca="1" si="2"/>
-        <v>549.7802576024493</v>
+        <v>549.1792767053098</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -22156,7 +22156,7 @@
       </c>
       <c r="B177">
         <f t="shared" ca="1" si="2"/>
-        <v>549.8495179235008</v>
+        <v>549.20602170067184</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -22165,7 +22165,7 @@
       </c>
       <c r="B178">
         <f t="shared" ca="1" si="2"/>
-        <v>549.94685081532782</v>
+        <v>549.25947285197617</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -22174,7 +22174,7 @@
       </c>
       <c r="B179">
         <f t="shared" ref="B179:B242" ca="1" si="3">B178+0.1*RAND()</f>
-        <v>549.97944081023934</v>
+        <v>549.30359973499947</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -22183,7 +22183,7 @@
       </c>
       <c r="B180">
         <f t="shared" ca="1" si="3"/>
-        <v>550.05753864905637</v>
+        <v>549.36615764331475</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -22192,7 +22192,7 @@
       </c>
       <c r="B181">
         <f t="shared" ca="1" si="3"/>
-        <v>550.10202955711748</v>
+        <v>549.39994563119751</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -22201,7 +22201,7 @@
       </c>
       <c r="B182">
         <f t="shared" ca="1" si="3"/>
-        <v>550.18809956113762</v>
+        <v>549.4196613436477</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -22210,7 +22210,7 @@
       </c>
       <c r="B183">
         <f t="shared" ca="1" si="3"/>
-        <v>550.19459243524727</v>
+        <v>549.49477687149556</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -22219,7 +22219,7 @@
       </c>
       <c r="B184">
         <f t="shared" ca="1" si="3"/>
-        <v>550.25470753108573</v>
+        <v>549.49977946527554</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -22228,7 +22228,7 @@
       </c>
       <c r="B185">
         <f t="shared" ca="1" si="3"/>
-        <v>550.31251743345501</v>
+        <v>549.5858583125414</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -22237,7 +22237,7 @@
       </c>
       <c r="B186">
         <f t="shared" ca="1" si="3"/>
-        <v>550.37269114416472</v>
+        <v>549.65731021265117</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -22246,7 +22246,7 @@
       </c>
       <c r="B187">
         <f t="shared" ca="1" si="3"/>
-        <v>550.45423393367014</v>
+        <v>549.7371820872155</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -22255,7 +22255,7 @@
       </c>
       <c r="B188">
         <f t="shared" ca="1" si="3"/>
-        <v>550.46595707655001</v>
+        <v>549.83490989185464</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -22264,7 +22264,7 @@
       </c>
       <c r="B189">
         <f t="shared" ca="1" si="3"/>
-        <v>550.46825239806697</v>
+        <v>549.92239079058038</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -22273,7 +22273,7 @@
       </c>
       <c r="B190">
         <f t="shared" ca="1" si="3"/>
-        <v>550.52443791459473</v>
+        <v>549.93450686211986</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -22282,7 +22282,7 @@
       </c>
       <c r="B191">
         <f t="shared" ca="1" si="3"/>
-        <v>550.55418992325792</v>
+        <v>550.03092618130859</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -22291,7 +22291,7 @@
       </c>
       <c r="B192">
         <f t="shared" ca="1" si="3"/>
-        <v>550.59376394048775</v>
+        <v>550.12182971024936</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -22300,7 +22300,7 @@
       </c>
       <c r="B193">
         <f t="shared" ca="1" si="3"/>
-        <v>550.68405514444794</v>
+        <v>550.16245128201865</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -22309,7 +22309,7 @@
       </c>
       <c r="B194">
         <f t="shared" ca="1" si="3"/>
-        <v>550.73731341909354</v>
+        <v>550.23859409075385</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -22318,7 +22318,7 @@
       </c>
       <c r="B195">
         <f t="shared" ca="1" si="3"/>
-        <v>550.75618403511919</v>
+        <v>550.25723325944523</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -22327,7 +22327,7 @@
       </c>
       <c r="B196">
         <f t="shared" ca="1" si="3"/>
-        <v>550.81249032080586</v>
+        <v>550.333562520795</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -22336,7 +22336,7 @@
       </c>
       <c r="B197">
         <f t="shared" ca="1" si="3"/>
-        <v>550.86211903378592</v>
+        <v>550.3345325981104</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -22345,7 +22345,7 @@
       </c>
       <c r="B198">
         <f t="shared" ca="1" si="3"/>
-        <v>550.94175678230056</v>
+        <v>550.39737714290425</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -22354,7 +22354,7 @@
       </c>
       <c r="B199">
         <f t="shared" ca="1" si="3"/>
-        <v>550.98946392882249</v>
+        <v>550.49434762993769</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -22363,7 +22363,7 @@
       </c>
       <c r="B200">
         <f t="shared" ca="1" si="3"/>
-        <v>551.06133503792216</v>
+        <v>550.53684807353773</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -22372,7 +22372,7 @@
       </c>
       <c r="B201">
         <f t="shared" ca="1" si="3"/>
-        <v>551.11560903665691</v>
+        <v>550.5518659643086</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -22381,7 +22381,7 @@
       </c>
       <c r="B202">
         <f t="shared" ca="1" si="3"/>
-        <v>551.15056145878407</v>
+        <v>550.59422475236966</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -22390,7 +22390,7 @@
       </c>
       <c r="B203">
         <f t="shared" ca="1" si="3"/>
-        <v>551.2247684464221</v>
+        <v>550.67378613913115</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -22399,7 +22399,7 @@
       </c>
       <c r="B204">
         <f t="shared" ca="1" si="3"/>
-        <v>551.29646599956664</v>
+        <v>550.7116778689192</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -22408,7 +22408,7 @@
       </c>
       <c r="B205">
         <f t="shared" ca="1" si="3"/>
-        <v>551.33558493614055</v>
+        <v>550.73142726890592</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -22417,7 +22417,7 @@
       </c>
       <c r="B206">
         <f t="shared" ca="1" si="3"/>
-        <v>551.33716164441648</v>
+        <v>550.77130087709622</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -22426,7 +22426,7 @@
       </c>
       <c r="B207">
         <f t="shared" ca="1" si="3"/>
-        <v>551.40877939252209</v>
+        <v>550.85572402467096</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -22435,7 +22435,7 @@
       </c>
       <c r="B208">
         <f t="shared" ca="1" si="3"/>
-        <v>551.44119284129272</v>
+        <v>550.88083849132317</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -22444,7 +22444,7 @@
       </c>
       <c r="B209">
         <f t="shared" ca="1" si="3"/>
-        <v>551.51408759137485</v>
+        <v>550.95614492098605</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -22453,7 +22453,7 @@
       </c>
       <c r="B210">
         <f t="shared" ca="1" si="3"/>
-        <v>551.52757371031203</v>
+        <v>550.95771777925449</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -22462,7 +22462,7 @@
       </c>
       <c r="B211">
         <f t="shared" ca="1" si="3"/>
-        <v>551.54019690505322</v>
+        <v>551.04731420575126</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -22471,7 +22471,7 @@
       </c>
       <c r="B212">
         <f t="shared" ca="1" si="3"/>
-        <v>551.59941984593809</v>
+        <v>551.06476009222422</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -22480,7 +22480,7 @@
       </c>
       <c r="B213">
         <f t="shared" ca="1" si="3"/>
-        <v>551.6142328980178</v>
+        <v>551.15422112145473</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -22489,7 +22489,7 @@
       </c>
       <c r="B214">
         <f t="shared" ca="1" si="3"/>
-        <v>551.66102941791439</v>
+        <v>551.18463258901102</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -22498,7 +22498,7 @@
       </c>
       <c r="B215">
         <f t="shared" ca="1" si="3"/>
-        <v>551.69908579319974</v>
+        <v>551.24297401367267</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -22507,7 +22507,7 @@
       </c>
       <c r="B216">
         <f t="shared" ca="1" si="3"/>
-        <v>551.70845276994316</v>
+        <v>551.28034071219793</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -22516,7 +22516,7 @@
       </c>
       <c r="B217">
         <f t="shared" ca="1" si="3"/>
-        <v>551.7431640486227</v>
+        <v>551.29974217855977</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -22525,7 +22525,7 @@
       </c>
       <c r="B218">
         <f t="shared" ca="1" si="3"/>
-        <v>551.79405893407466</v>
+        <v>551.30592085063859</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -22534,7 +22534,7 @@
       </c>
       <c r="B219">
         <f t="shared" ca="1" si="3"/>
-        <v>551.80114488713184</v>
+        <v>551.40265304790444</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -22543,7 +22543,7 @@
       </c>
       <c r="B220">
         <f t="shared" ca="1" si="3"/>
-        <v>551.89410945275108</v>
+        <v>551.44665924345566</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -22552,7 +22552,7 @@
       </c>
       <c r="B221">
         <f t="shared" ca="1" si="3"/>
-        <v>551.98950967111557</v>
+        <v>551.47155020369928</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -22561,7 +22561,7 @@
       </c>
       <c r="B222">
         <f t="shared" ca="1" si="3"/>
-        <v>552.05913307518028</v>
+        <v>551.51039637473434</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -22570,7 +22570,7 @@
       </c>
       <c r="B223">
         <f t="shared" ca="1" si="3"/>
-        <v>552.13835893457031</v>
+        <v>551.57804443821669</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -22579,7 +22579,7 @@
       </c>
       <c r="B224">
         <f t="shared" ca="1" si="3"/>
-        <v>552.19725944399852</v>
+        <v>551.61085890888376</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -22588,7 +22588,7 @@
       </c>
       <c r="B225">
         <f t="shared" ca="1" si="3"/>
-        <v>552.27988987405547</v>
+        <v>551.67887782472758</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -22597,7 +22597,7 @@
       </c>
       <c r="B226">
         <f t="shared" ca="1" si="3"/>
-        <v>552.3700819167359</v>
+        <v>551.72446213957608</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -22606,7 +22606,7 @@
       </c>
       <c r="B227">
         <f t="shared" ca="1" si="3"/>
-        <v>552.4491194278869</v>
+        <v>551.78342449186607</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -22615,7 +22615,7 @@
       </c>
       <c r="B228">
         <f t="shared" ca="1" si="3"/>
-        <v>552.45018446677545</v>
+        <v>551.87807823255309</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -22624,7 +22624,7 @@
       </c>
       <c r="B229">
         <f t="shared" ca="1" si="3"/>
-        <v>552.5176035529305</v>
+        <v>551.90410482165396</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -22633,7 +22633,7 @@
       </c>
       <c r="B230">
         <f t="shared" ca="1" si="3"/>
-        <v>552.61061897811362</v>
+        <v>551.94722582104498</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -22642,7 +22642,7 @@
       </c>
       <c r="B231">
         <f t="shared" ca="1" si="3"/>
-        <v>552.6337010622583</v>
+        <v>551.97594226586773</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -22651,7 +22651,7 @@
       </c>
       <c r="B232">
         <f t="shared" ca="1" si="3"/>
-        <v>552.71402441930047</v>
+        <v>552.07393521760434</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -22660,7 +22660,7 @@
       </c>
       <c r="B233">
         <f t="shared" ca="1" si="3"/>
-        <v>552.79085289477507</v>
+        <v>552.15974498809305</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -22669,7 +22669,7 @@
       </c>
       <c r="B234">
         <f t="shared" ca="1" si="3"/>
-        <v>552.83532815532578</v>
+        <v>552.19736657338137</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -22678,7 +22678,7 @@
       </c>
       <c r="B235">
         <f t="shared" ca="1" si="3"/>
-        <v>552.89952009334411</v>
+        <v>552.19963061847261</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -22687,7 +22687,7 @@
       </c>
       <c r="B236">
         <f t="shared" ca="1" si="3"/>
-        <v>552.93555525497516</v>
+        <v>552.26856729195106</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -22696,7 +22696,7 @@
       </c>
       <c r="B237">
         <f t="shared" ca="1" si="3"/>
-        <v>552.96353302997068</v>
+        <v>552.30626129921779</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -22705,7 +22705,7 @@
       </c>
       <c r="B238">
         <f t="shared" ca="1" si="3"/>
-        <v>553.00020659128279</v>
+        <v>552.30758505784752</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -22714,7 +22714,7 @@
       </c>
       <c r="B239">
         <f t="shared" ca="1" si="3"/>
-        <v>553.03441007639708</v>
+        <v>552.33664538115886</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -22723,7 +22723,7 @@
       </c>
       <c r="B240">
         <f t="shared" ca="1" si="3"/>
-        <v>553.09700555237316</v>
+        <v>552.43533312486113</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -22732,7 +22732,7 @@
       </c>
       <c r="B241">
         <f t="shared" ca="1" si="3"/>
-        <v>553.15166775599619</v>
+        <v>552.53215967424126</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
@@ -22741,7 +22741,7 @@
       </c>
       <c r="B242">
         <f t="shared" ca="1" si="3"/>
-        <v>553.21005073112167</v>
+        <v>552.59435833108103</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -22750,7 +22750,7 @@
       </c>
       <c r="B243">
         <f t="shared" ref="B243:B306" ca="1" si="4">B242+0.1*RAND()</f>
-        <v>553.24379717713077</v>
+        <v>552.66590898887398</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -22759,7 +22759,7 @@
       </c>
       <c r="B244">
         <f t="shared" ca="1" si="4"/>
-        <v>553.25965437908962</v>
+        <v>552.74299714471317</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -22768,7 +22768,7 @@
       </c>
       <c r="B245">
         <f t="shared" ca="1" si="4"/>
-        <v>553.27619093847852</v>
+        <v>552.79794844883895</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -22777,7 +22777,7 @@
       </c>
       <c r="B246">
         <f t="shared" ca="1" si="4"/>
-        <v>553.29707012334757</v>
+        <v>552.83180761471272</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -22786,7 +22786,7 @@
       </c>
       <c r="B247">
         <f t="shared" ca="1" si="4"/>
-        <v>553.35399330944131</v>
+        <v>552.85088670928519</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -22795,7 +22795,7 @@
       </c>
       <c r="B248">
         <f t="shared" ca="1" si="4"/>
-        <v>553.3734001832679</v>
+        <v>552.93842770763661</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -22804,7 +22804,7 @@
       </c>
       <c r="B249">
         <f t="shared" ca="1" si="4"/>
-        <v>553.47317886721828</v>
+        <v>552.94197658976941</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -22813,7 +22813,7 @@
       </c>
       <c r="B250">
         <f t="shared" ca="1" si="4"/>
-        <v>553.49341399892887</v>
+        <v>553.00834401586485</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -22822,7 +22822,7 @@
       </c>
       <c r="B251">
         <f t="shared" ca="1" si="4"/>
-        <v>553.52032600597784</v>
+        <v>553.10720163331632</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -22831,7 +22831,7 @@
       </c>
       <c r="B252">
         <f t="shared" ca="1" si="4"/>
-        <v>553.52383005862066</v>
+        <v>553.15479033789836</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -22840,7 +22840,7 @@
       </c>
       <c r="B253">
         <f t="shared" ca="1" si="4"/>
-        <v>553.58454585514858</v>
+        <v>553.18831635932906</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -22849,7 +22849,7 @@
       </c>
       <c r="B254">
         <f t="shared" ca="1" si="4"/>
-        <v>553.63242781063695</v>
+        <v>553.24796339094087</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
@@ -22858,7 +22858,7 @@
       </c>
       <c r="B255">
         <f t="shared" ca="1" si="4"/>
-        <v>553.64055688575513</v>
+        <v>553.26893949423356</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -22867,7 +22867,7 @@
       </c>
       <c r="B256">
         <f t="shared" ca="1" si="4"/>
-        <v>553.71273470998074</v>
+        <v>553.28149685269454</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -22876,7 +22876,7 @@
       </c>
       <c r="B257">
         <f t="shared" ca="1" si="4"/>
-        <v>553.79036436806769</v>
+        <v>553.28958651086987</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
@@ -22885,7 +22885,7 @@
       </c>
       <c r="B258">
         <f t="shared" ca="1" si="4"/>
-        <v>553.88815963311595</v>
+        <v>553.31079894846505</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -22894,7 +22894,7 @@
       </c>
       <c r="B259">
         <f t="shared" ca="1" si="4"/>
-        <v>553.9147098615382</v>
+        <v>553.35301707714552</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -22903,7 +22903,7 @@
       </c>
       <c r="B260">
         <f t="shared" ca="1" si="4"/>
-        <v>553.96687782512038</v>
+        <v>553.40642653458167</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -22912,7 +22912,7 @@
       </c>
       <c r="B261">
         <f t="shared" ca="1" si="4"/>
-        <v>553.98197862091934</v>
+        <v>553.41739568122227</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
@@ -22921,7 +22921,7 @@
       </c>
       <c r="B262">
         <f t="shared" ca="1" si="4"/>
-        <v>554.05562126661528</v>
+        <v>553.42866485305422</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
@@ -22930,7 +22930,7 @@
       </c>
       <c r="B263">
         <f t="shared" ca="1" si="4"/>
-        <v>554.12223681007981</v>
+        <v>553.51757156516646</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -22939,7 +22939,7 @@
       </c>
       <c r="B264">
         <f t="shared" ca="1" si="4"/>
-        <v>554.12717848867442</v>
+        <v>553.55530654175368</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -22948,7 +22948,7 @@
       </c>
       <c r="B265">
         <f t="shared" ca="1" si="4"/>
-        <v>554.22636319175149</v>
+        <v>553.61485122289287</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
@@ -22957,7 +22957,7 @@
       </c>
       <c r="B266">
         <f t="shared" ca="1" si="4"/>
-        <v>554.27532743546158</v>
+        <v>553.67471438707275</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
@@ -22966,7 +22966,7 @@
       </c>
       <c r="B267">
         <f t="shared" ca="1" si="4"/>
-        <v>554.30849296748249</v>
+        <v>553.73005914713531</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -22975,7 +22975,7 @@
       </c>
       <c r="B268">
         <f t="shared" ca="1" si="4"/>
-        <v>554.34351917149104</v>
+        <v>553.74078004704177</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
@@ -22984,7 +22984,7 @@
       </c>
       <c r="B269">
         <f t="shared" ca="1" si="4"/>
-        <v>554.36763868960952</v>
+        <v>553.74952550628427</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
@@ -22993,7 +22993,7 @@
       </c>
       <c r="B270">
         <f t="shared" ca="1" si="4"/>
-        <v>554.45001190305481</v>
+        <v>553.81385405494166</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -23002,7 +23002,7 @@
       </c>
       <c r="B271">
         <f t="shared" ca="1" si="4"/>
-        <v>554.47248910565861</v>
+        <v>553.8509976427988</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
@@ -23011,7 +23011,7 @@
       </c>
       <c r="B272">
         <f t="shared" ca="1" si="4"/>
-        <v>554.57024595679502</v>
+        <v>553.93708538076669</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
@@ -23020,7 +23020,7 @@
       </c>
       <c r="B273">
         <f t="shared" ca="1" si="4"/>
-        <v>554.61952778151203</v>
+        <v>553.98322325153561</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
@@ -23029,7 +23029,7 @@
       </c>
       <c r="B274">
         <f t="shared" ca="1" si="4"/>
-        <v>554.71897091629171</v>
+        <v>554.03381590512549</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
@@ -23038,7 +23038,7 @@
       </c>
       <c r="B275">
         <f t="shared" ca="1" si="4"/>
-        <v>554.81442328451749</v>
+        <v>554.11901826183259</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
@@ -23047,7 +23047,7 @@
       </c>
       <c r="B276">
         <f t="shared" ca="1" si="4"/>
-        <v>554.89977627009682</v>
+        <v>554.18095719505254</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
@@ -23056,7 +23056,7 @@
       </c>
       <c r="B277">
         <f t="shared" ca="1" si="4"/>
-        <v>554.99809323819068</v>
+        <v>554.23019763598018</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
@@ -23065,7 +23065,7 @@
       </c>
       <c r="B278">
         <f t="shared" ca="1" si="4"/>
-        <v>555.03223732912056</v>
+        <v>554.32543028033695</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
@@ -23074,7 +23074,7 @@
       </c>
       <c r="B279">
         <f t="shared" ca="1" si="4"/>
-        <v>555.10086509123153</v>
+        <v>554.39145279300578</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -23083,7 +23083,7 @@
       </c>
       <c r="B280">
         <f t="shared" ca="1" si="4"/>
-        <v>555.1024001405118</v>
+        <v>554.43584717734109</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
@@ -23092,7 +23092,7 @@
       </c>
       <c r="B281">
         <f t="shared" ca="1" si="4"/>
-        <v>555.12353218482974</v>
+        <v>554.50386077849009</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
@@ -23101,7 +23101,7 @@
       </c>
       <c r="B282">
         <f t="shared" ca="1" si="4"/>
-        <v>555.19011440559154</v>
+        <v>554.5305132597299</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -23110,7 +23110,7 @@
       </c>
       <c r="B283">
         <f t="shared" ca="1" si="4"/>
-        <v>555.23481674434925</v>
+        <v>554.56251313941505</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
@@ -23119,7 +23119,7 @@
       </c>
       <c r="B284">
         <f t="shared" ca="1" si="4"/>
-        <v>555.23567806652181</v>
+        <v>554.6392040213874</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
@@ -23128,7 +23128,7 @@
       </c>
       <c r="B285">
         <f t="shared" ca="1" si="4"/>
-        <v>555.29331342865817</v>
+        <v>554.65716381592154</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
@@ -23137,7 +23137,7 @@
       </c>
       <c r="B286">
         <f t="shared" ca="1" si="4"/>
-        <v>555.31022297116931</v>
+        <v>554.6943571248172</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
@@ -23146,7 +23146,7 @@
       </c>
       <c r="B287">
         <f t="shared" ca="1" si="4"/>
-        <v>555.38576553573978</v>
+        <v>554.77746857361365</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
@@ -23155,7 +23155,7 @@
       </c>
       <c r="B288">
         <f t="shared" ca="1" si="4"/>
-        <v>555.44034965848948</v>
+        <v>554.82261726211004</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
@@ -23164,7 +23164,7 @@
       </c>
       <c r="B289">
         <f t="shared" ca="1" si="4"/>
-        <v>555.51066488687513</v>
+        <v>554.86909571564956</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
@@ -23173,7 +23173,7 @@
       </c>
       <c r="B290">
         <f t="shared" ca="1" si="4"/>
-        <v>555.5215743491076</v>
+        <v>554.91700261150515</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
@@ -23182,7 +23182,7 @@
       </c>
       <c r="B291">
         <f t="shared" ca="1" si="4"/>
-        <v>555.5290734195105</v>
+        <v>554.92285766237626</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
@@ -23191,7 +23191,7 @@
       </c>
       <c r="B292">
         <f t="shared" ca="1" si="4"/>
-        <v>555.59386942645096</v>
+        <v>554.92885936113805</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
@@ -23200,7 +23200,7 @@
       </c>
       <c r="B293">
         <f t="shared" ca="1" si="4"/>
-        <v>555.61624997009358</v>
+        <v>554.95094173232565</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
@@ -23209,7 +23209,7 @@
       </c>
       <c r="B294">
         <f t="shared" ca="1" si="4"/>
-        <v>555.63779171772012</v>
+        <v>555.04205683668147</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -23218,7 +23218,7 @@
       </c>
       <c r="B295">
         <f t="shared" ca="1" si="4"/>
-        <v>555.69305111947983</v>
+        <v>555.09822880628531</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
@@ -23227,7 +23227,7 @@
       </c>
       <c r="B296">
         <f t="shared" ca="1" si="4"/>
-        <v>555.79161622542586</v>
+        <v>555.11962862029566</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
@@ -23236,7 +23236,7 @@
       </c>
       <c r="B297">
         <f t="shared" ca="1" si="4"/>
-        <v>555.80048519750915</v>
+        <v>555.18686259182675</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -23245,7 +23245,7 @@
       </c>
       <c r="B298">
         <f t="shared" ca="1" si="4"/>
-        <v>555.85007291652289</v>
+        <v>555.26499502501713</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -23254,7 +23254,7 @@
       </c>
       <c r="B299">
         <f t="shared" ca="1" si="4"/>
-        <v>555.88116699551369</v>
+        <v>555.36287231954964</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
@@ -23263,7 +23263,7 @@
       </c>
       <c r="B300">
         <f t="shared" ca="1" si="4"/>
-        <v>555.97782119093972</v>
+        <v>555.3743068798675</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -23272,7 +23272,7 @@
       </c>
       <c r="B301">
         <f t="shared" ca="1" si="4"/>
-        <v>556.04190814234369</v>
+        <v>555.45088141546682</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
@@ -23281,7 +23281,7 @@
       </c>
       <c r="B302">
         <f t="shared" ca="1" si="4"/>
-        <v>556.12911006106549</v>
+        <v>555.47299417604563</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
@@ -23290,7 +23290,7 @@
       </c>
       <c r="B303">
         <f t="shared" ca="1" si="4"/>
-        <v>556.19622429272044</v>
+        <v>555.50767801976224</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -23299,7 +23299,7 @@
       </c>
       <c r="B304">
         <f t="shared" ca="1" si="4"/>
-        <v>556.21279484668344</v>
+        <v>555.56676008004763</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -23308,7 +23308,7 @@
       </c>
       <c r="B305">
         <f t="shared" ca="1" si="4"/>
-        <v>556.21795767775177</v>
+        <v>555.58911237655718</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
@@ -23317,7 +23317,7 @@
       </c>
       <c r="B306">
         <f t="shared" ca="1" si="4"/>
-        <v>556.24357336055607</v>
+        <v>555.67611395333211</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -23326,7 +23326,7 @@
       </c>
       <c r="B307">
         <f t="shared" ref="B307:B370" ca="1" si="5">B306+0.1*RAND()</f>
-        <v>556.25662398576083</v>
+        <v>555.72669237500952</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
@@ -23335,7 +23335,7 @@
       </c>
       <c r="B308">
         <f t="shared" ca="1" si="5"/>
-        <v>556.30934254083002</v>
+        <v>555.81438464862276</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
@@ -23344,7 +23344,7 @@
       </c>
       <c r="B309">
         <f t="shared" ca="1" si="5"/>
-        <v>556.36596440069434</v>
+        <v>555.85392563816902</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -23353,7 +23353,7 @@
       </c>
       <c r="B310">
         <f t="shared" ca="1" si="5"/>
-        <v>556.41098099027067</v>
+        <v>555.90765168450878</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
@@ -23362,7 +23362,7 @@
       </c>
       <c r="B311">
         <f t="shared" ca="1" si="5"/>
-        <v>556.49056841044887</v>
+        <v>555.9644049552852</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
@@ -23371,7 +23371,7 @@
       </c>
       <c r="B312">
         <f t="shared" ca="1" si="5"/>
-        <v>556.51159508679075</v>
+        <v>556.0207979700125</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -23380,7 +23380,7 @@
       </c>
       <c r="B313">
         <f t="shared" ca="1" si="5"/>
-        <v>556.53058330740657</v>
+        <v>556.08594843068363</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
@@ -23389,7 +23389,7 @@
       </c>
       <c r="B314">
         <f t="shared" ca="1" si="5"/>
-        <v>556.61895924071246</v>
+        <v>556.08882881569195</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
@@ -23398,7 +23398,7 @@
       </c>
       <c r="B315">
         <f t="shared" ca="1" si="5"/>
-        <v>556.69006555830538</v>
+        <v>556.14619693787745</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -23407,7 +23407,7 @@
       </c>
       <c r="B316">
         <f t="shared" ca="1" si="5"/>
-        <v>556.77001778768704</v>
+        <v>556.1679279483842</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
@@ -23416,7 +23416,7 @@
       </c>
       <c r="B317">
         <f t="shared" ca="1" si="5"/>
-        <v>556.86825843612348</v>
+        <v>556.20003141174448</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
@@ -23425,7 +23425,7 @@
       </c>
       <c r="B318">
         <f t="shared" ca="1" si="5"/>
-        <v>556.93391926039305</v>
+        <v>556.28213677503118</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -23434,7 +23434,7 @@
       </c>
       <c r="B319">
         <f t="shared" ca="1" si="5"/>
-        <v>556.94849575294541</v>
+        <v>556.34963271546462</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
@@ -23443,7 +23443,7 @@
       </c>
       <c r="B320">
         <f t="shared" ca="1" si="5"/>
-        <v>556.95139759198344</v>
+        <v>556.36565697137837</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
@@ -23452,7 +23452,7 @@
       </c>
       <c r="B321">
         <f t="shared" ca="1" si="5"/>
-        <v>556.98540050018198</v>
+        <v>556.45399833472084</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -23461,7 +23461,7 @@
       </c>
       <c r="B322">
         <f t="shared" ca="1" si="5"/>
-        <v>557.02796351259849</v>
+        <v>556.46878288852179</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
@@ -23470,7 +23470,7 @@
       </c>
       <c r="B323">
         <f t="shared" ca="1" si="5"/>
-        <v>557.05966332449441</v>
+        <v>556.55557685870406</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
@@ -23479,7 +23479,7 @@
       </c>
       <c r="B324">
         <f t="shared" ca="1" si="5"/>
-        <v>557.12845514447395</v>
+        <v>556.61306056252317</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -23488,7 +23488,7 @@
       </c>
       <c r="B325">
         <f t="shared" ca="1" si="5"/>
-        <v>557.14325777265663</v>
+        <v>556.64686019763894</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
@@ -23497,7 +23497,7 @@
       </c>
       <c r="B326">
         <f t="shared" ca="1" si="5"/>
-        <v>557.14503813255828</v>
+        <v>556.70941809188867</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
@@ -23506,7 +23506,7 @@
       </c>
       <c r="B327">
         <f t="shared" ca="1" si="5"/>
-        <v>557.21076442821914</v>
+        <v>556.77341257841931</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
@@ -23515,7 +23515,7 @@
       </c>
       <c r="B328">
         <f t="shared" ca="1" si="5"/>
-        <v>557.27465046554425</v>
+        <v>556.78690549071064</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
@@ -23524,7 +23524,7 @@
       </c>
       <c r="B329">
         <f t="shared" ca="1" si="5"/>
-        <v>557.31009475972019</v>
+        <v>556.81536852652164</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
@@ -23533,7 +23533,7 @@
       </c>
       <c r="B330">
         <f t="shared" ca="1" si="5"/>
-        <v>557.40729970222515</v>
+        <v>556.83297776477082</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -23542,7 +23542,7 @@
       </c>
       <c r="B331">
         <f t="shared" ca="1" si="5"/>
-        <v>557.43194263958651</v>
+        <v>556.88086262066463</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
@@ -23551,7 +23551,7 @@
       </c>
       <c r="B332">
         <f t="shared" ca="1" si="5"/>
-        <v>557.46043398490372</v>
+        <v>556.89692963120774</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
@@ -23560,7 +23560,7 @@
       </c>
       <c r="B333">
         <f t="shared" ca="1" si="5"/>
-        <v>557.54120845187913</v>
+        <v>556.97347405985579</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -23569,7 +23569,7 @@
       </c>
       <c r="B334">
         <f t="shared" ca="1" si="5"/>
-        <v>557.57206563531327</v>
+        <v>556.98973290580329</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
@@ -23578,7 +23578,7 @@
       </c>
       <c r="B335">
         <f t="shared" ca="1" si="5"/>
-        <v>557.60180908956193</v>
+        <v>557.03598698994881</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
@@ -23587,7 +23587,7 @@
       </c>
       <c r="B336">
         <f t="shared" ca="1" si="5"/>
-        <v>557.65341046507933</v>
+        <v>557.06381109329425</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
@@ -23596,7 +23596,7 @@
       </c>
       <c r="B337">
         <f t="shared" ca="1" si="5"/>
-        <v>557.73959254664317</v>
+        <v>557.0795814449308</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
@@ -23605,7 +23605,7 @@
       </c>
       <c r="B338">
         <f t="shared" ca="1" si="5"/>
-        <v>557.82071511342451</v>
+        <v>557.11453817196548</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
@@ -23614,7 +23614,7 @@
       </c>
       <c r="B339">
         <f t="shared" ca="1" si="5"/>
-        <v>557.82652550456942</v>
+        <v>557.20346711445791</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
@@ -23623,7 +23623,7 @@
       </c>
       <c r="B340">
         <f t="shared" ca="1" si="5"/>
-        <v>557.85188579681221</v>
+        <v>557.26416287994368</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
@@ -23632,7 +23632,7 @@
       </c>
       <c r="B341">
         <f t="shared" ca="1" si="5"/>
-        <v>557.94465307945893</v>
+        <v>557.32402521534675</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
@@ -23641,7 +23641,7 @@
       </c>
       <c r="B342">
         <f t="shared" ca="1" si="5"/>
-        <v>558.03443187840912</v>
+        <v>557.39800648794915</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -23650,7 +23650,7 @@
       </c>
       <c r="B343">
         <f t="shared" ca="1" si="5"/>
-        <v>558.06333248711235</v>
+        <v>557.46800342087374</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
@@ -23659,7 +23659,7 @@
       </c>
       <c r="B344">
         <f t="shared" ca="1" si="5"/>
-        <v>558.12781903114478</v>
+        <v>557.56095779179657</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
@@ -23668,7 +23668,7 @@
       </c>
       <c r="B345">
         <f t="shared" ca="1" si="5"/>
-        <v>558.18166604787609</v>
+        <v>557.63549716291459</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -23677,7 +23677,7 @@
       </c>
       <c r="B346">
         <f t="shared" ca="1" si="5"/>
-        <v>558.22433994259859</v>
+        <v>557.65714319142</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
@@ -23686,7 +23686,7 @@
       </c>
       <c r="B347">
         <f t="shared" ca="1" si="5"/>
-        <v>558.2325164550814</v>
+        <v>557.68844153458042</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
@@ -23695,7 +23695,7 @@
       </c>
       <c r="B348">
         <f t="shared" ca="1" si="5"/>
-        <v>558.30286179552354</v>
+        <v>557.76650971900051</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -23704,7 +23704,7 @@
       </c>
       <c r="B349">
         <f t="shared" ca="1" si="5"/>
-        <v>558.38543845200445</v>
+        <v>557.81121072407495</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
@@ -23713,7 +23713,7 @@
       </c>
       <c r="B350">
         <f t="shared" ca="1" si="5"/>
-        <v>558.44313391809692</v>
+        <v>557.81827496343215</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
@@ -23722,7 +23722,7 @@
       </c>
       <c r="B351">
         <f t="shared" ca="1" si="5"/>
-        <v>558.50101999180981</v>
+        <v>557.85089282069623</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
@@ -23731,7 +23731,7 @@
       </c>
       <c r="B352">
         <f t="shared" ca="1" si="5"/>
-        <v>558.50349257175287</v>
+        <v>557.94808022591462</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
@@ -23740,7 +23740,7 @@
       </c>
       <c r="B353">
         <f t="shared" ca="1" si="5"/>
-        <v>558.52108628673022</v>
+        <v>557.973503312807</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
@@ -23749,7 +23749,7 @@
       </c>
       <c r="B354">
         <f t="shared" ca="1" si="5"/>
-        <v>558.61435598561036</v>
+        <v>558.01941879829235</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
@@ -23758,7 +23758,7 @@
       </c>
       <c r="B355">
         <f t="shared" ca="1" si="5"/>
-        <v>558.64970711002593</v>
+        <v>558.09966524588435</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
@@ -23767,7 +23767,7 @@
       </c>
       <c r="B356">
         <f t="shared" ca="1" si="5"/>
-        <v>558.68248640710874</v>
+        <v>558.17695417054983</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
@@ -23776,7 +23776,7 @@
       </c>
       <c r="B357">
         <f t="shared" ca="1" si="5"/>
-        <v>558.76753614551922</v>
+        <v>558.22010979158927</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -23785,7 +23785,7 @@
       </c>
       <c r="B358">
         <f t="shared" ca="1" si="5"/>
-        <v>558.78070586830097</v>
+        <v>558.31328783502386</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
@@ -23794,7 +23794,7 @@
       </c>
       <c r="B359">
         <f t="shared" ca="1" si="5"/>
-        <v>558.872150019223</v>
+        <v>558.34125254300818</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
@@ -23803,7 +23803,7 @@
       </c>
       <c r="B360">
         <f t="shared" ca="1" si="5"/>
-        <v>558.87459459127945</v>
+        <v>558.37573059487408</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
@@ -23812,7 +23812,7 @@
       </c>
       <c r="B361">
         <f t="shared" ca="1" si="5"/>
-        <v>558.92226891758571</v>
+        <v>558.45719722114086</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
@@ -23821,7 +23821,7 @@
       </c>
       <c r="B362">
         <f t="shared" ca="1" si="5"/>
-        <v>559.01155617657048</v>
+        <v>558.4840924756046</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
@@ -23830,7 +23830,7 @@
       </c>
       <c r="B363">
         <f t="shared" ca="1" si="5"/>
-        <v>559.04948498318629</v>
+        <v>558.52989152693613</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
@@ -23839,7 +23839,7 @@
       </c>
       <c r="B364">
         <f t="shared" ca="1" si="5"/>
-        <v>559.11745781509876</v>
+        <v>558.53992239477736</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
@@ -23848,7 +23848,7 @@
       </c>
       <c r="B365">
         <f t="shared" ca="1" si="5"/>
-        <v>559.15730468694028</v>
+        <v>558.56245400363173</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
@@ -23857,7 +23857,7 @@
       </c>
       <c r="B366">
         <f t="shared" ca="1" si="5"/>
-        <v>559.16976062669391</v>
+        <v>558.61965598227471</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
@@ -23866,7 +23866,7 @@
       </c>
       <c r="B367">
         <f t="shared" ca="1" si="5"/>
-        <v>559.1803024888037</v>
+        <v>558.71754059541058</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
@@ -23875,7 +23875,7 @@
       </c>
       <c r="B368">
         <f t="shared" ca="1" si="5"/>
-        <v>559.27350907481355</v>
+        <v>558.79399611274732</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
@@ -23884,7 +23884,7 @@
       </c>
       <c r="B369">
         <f t="shared" ca="1" si="5"/>
-        <v>559.30844673244644</v>
+        <v>558.84835502333158</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
@@ -23893,7 +23893,7 @@
       </c>
       <c r="B370">
         <f t="shared" ca="1" si="5"/>
-        <v>559.31214827275721</v>
+        <v>558.91894506118024</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
@@ -23902,7 +23902,7 @@
       </c>
       <c r="B371">
         <f t="shared" ref="B371:B402" ca="1" si="6">B370+0.1*RAND()</f>
-        <v>559.32954301252551</v>
+        <v>559.01172835190198</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
@@ -23911,7 +23911,7 @@
       </c>
       <c r="B372">
         <f t="shared" ca="1" si="6"/>
-        <v>559.3844932313142</v>
+        <v>559.08489885078131</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
@@ -23920,7 +23920,7 @@
       </c>
       <c r="B373">
         <f t="shared" ca="1" si="6"/>
-        <v>559.42301483486642</v>
+        <v>559.11193157769617</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
@@ -23929,7 +23929,7 @@
       </c>
       <c r="B374">
         <f t="shared" ca="1" si="6"/>
-        <v>559.50290382754599</v>
+        <v>559.17797467396213</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
@@ -23938,7 +23938,7 @@
       </c>
       <c r="B375">
         <f t="shared" ca="1" si="6"/>
-        <v>559.58085557105801</v>
+        <v>559.20994954131595</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -23947,7 +23947,7 @@
       </c>
       <c r="B376">
         <f t="shared" ca="1" si="6"/>
-        <v>559.60600096080395</v>
+        <v>559.30376303765911</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
@@ -23956,7 +23956,7 @@
       </c>
       <c r="B377">
         <f t="shared" ca="1" si="6"/>
-        <v>559.67826628991349</v>
+        <v>559.37975739374758</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
@@ -23965,7 +23965,7 @@
       </c>
       <c r="B378">
         <f t="shared" ca="1" si="6"/>
-        <v>559.69608768141336</v>
+        <v>559.46043225539677</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
@@ -23974,7 +23974,7 @@
       </c>
       <c r="B379">
         <f t="shared" ca="1" si="6"/>
-        <v>559.74169492302815</v>
+        <v>559.50684588658635</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
@@ -23983,7 +23983,7 @@
       </c>
       <c r="B380">
         <f t="shared" ca="1" si="6"/>
-        <v>559.83518917863842</v>
+        <v>559.54228641538407</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
@@ -23992,7 +23992,7 @@
       </c>
       <c r="B381">
         <f t="shared" ca="1" si="6"/>
-        <v>559.89731167495347</v>
+        <v>559.54278924354855</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
@@ -24001,7 +24001,7 @@
       </c>
       <c r="B382">
         <f t="shared" ca="1" si="6"/>
-        <v>559.95056275595562</v>
+        <v>559.6410420183571</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
@@ -24010,7 +24010,7 @@
       </c>
       <c r="B383">
         <f t="shared" ca="1" si="6"/>
-        <v>559.97886939398325</v>
+        <v>559.68926103443368</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
@@ -24019,7 +24019,7 @@
       </c>
       <c r="B384">
         <f t="shared" ca="1" si="6"/>
-        <v>559.98012886091249</v>
+        <v>559.69997299577449</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
@@ -24028,7 +24028,7 @@
       </c>
       <c r="B385">
         <f t="shared" ca="1" si="6"/>
-        <v>560.02077006271657</v>
+        <v>559.70195845373507</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
@@ -24037,7 +24037,7 @@
       </c>
       <c r="B386">
         <f t="shared" ca="1" si="6"/>
-        <v>560.05471651704579</v>
+        <v>559.71886679285581</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
@@ -24046,7 +24046,7 @@
       </c>
       <c r="B387">
         <f t="shared" ca="1" si="6"/>
-        <v>560.12540602051979</v>
+        <v>559.79357432426332</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
@@ -24055,7 +24055,7 @@
       </c>
       <c r="B388">
         <f t="shared" ca="1" si="6"/>
-        <v>560.14716441480687</v>
+        <v>559.88094090264042</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
@@ -24064,7 +24064,7 @@
       </c>
       <c r="B389">
         <f t="shared" ca="1" si="6"/>
-        <v>560.18636509217083</v>
+        <v>559.96042799870645</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
@@ -24073,7 +24073,7 @@
       </c>
       <c r="B390">
         <f t="shared" ca="1" si="6"/>
-        <v>560.22400165649788</v>
+        <v>560.06024392655115</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
@@ -24082,7 +24082,7 @@
       </c>
       <c r="B391">
         <f t="shared" ca="1" si="6"/>
-        <v>560.238420759679</v>
+        <v>560.14297613675058</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
@@ -24091,7 +24091,7 @@
       </c>
       <c r="B392">
         <f t="shared" ca="1" si="6"/>
-        <v>560.23957450622447</v>
+        <v>560.20856795313705</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
@@ -24100,7 +24100,7 @@
       </c>
       <c r="B393">
         <f t="shared" ca="1" si="6"/>
-        <v>560.27493193170972</v>
+        <v>560.23544904730375</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
@@ -24109,7 +24109,7 @@
       </c>
       <c r="B394">
         <f t="shared" ca="1" si="6"/>
-        <v>560.35546207311904</v>
+        <v>560.27759809416693</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
@@ -24118,7 +24118,7 @@
       </c>
       <c r="B395">
         <f t="shared" ca="1" si="6"/>
-        <v>560.43356950934935</v>
+        <v>560.29179498379881</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
@@ -24127,7 +24127,7 @@
       </c>
       <c r="B396">
         <f t="shared" ca="1" si="6"/>
-        <v>560.44998178536196</v>
+        <v>560.37522966858205</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
@@ -24136,7 +24136,7 @@
       </c>
       <c r="B397">
         <f t="shared" ca="1" si="6"/>
-        <v>560.47046585983537</v>
+        <v>560.44595028710853</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
@@ -24145,7 +24145,7 @@
       </c>
       <c r="B398">
         <f t="shared" ca="1" si="6"/>
-        <v>560.4801959390735</v>
+        <v>560.49203546050876</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
@@ -24154,7 +24154,7 @@
       </c>
       <c r="B399">
         <f t="shared" ca="1" si="6"/>
-        <v>560.48266041220222</v>
+        <v>560.56938535514894</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
@@ -24163,7 +24163,7 @@
       </c>
       <c r="B400">
         <f t="shared" ca="1" si="6"/>
-        <v>560.56739424225975</v>
+        <v>560.56972858350161</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
@@ -24172,7 +24172,7 @@
       </c>
       <c r="B401">
         <f t="shared" ca="1" si="6"/>
-        <v>560.66241157699119</v>
+        <v>560.58313154274958</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
@@ -24181,7 +24181,7 @@
       </c>
       <c r="B402">
         <f t="shared" ca="1" si="6"/>
-        <v>560.70370306233758</v>
+        <v>560.61896738001894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Islanded logic changes working (loSOC prompts diesel to turn on) "
</commit_message>
<xml_diff>
--- a/CART dependencies/Microgrid_cmd.xlsx
+++ b/CART dependencies/Microgrid_cmd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Autonomous-Microgrid-Control-with-Forecasting\CART dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B39DE5-092E-45D7-9192-67B7FD66F77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8338241-CC3A-4974-88A1-2B8796ECC501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
   </bookViews>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43E032D-C64D-4416-8490-73EE1F87088C}">
   <dimension ref="A1:B452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B22:B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +416,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -424,7 +424,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -432,7 +432,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -440,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -456,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -472,7 +472,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -488,7 +488,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -512,7 +512,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,7 +520,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,7 +528,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -544,7 +544,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -560,7 +560,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -576,7 +576,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -584,7 +584,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -600,7 +600,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -632,7 +632,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -640,7 +640,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -656,7 +656,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -680,7 +680,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -688,7 +688,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -696,7 +696,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -704,7 +704,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -728,7 +728,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -736,7 +736,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -744,7 +744,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,7 +768,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -792,7 +792,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2428,8 +2428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285FC894-56ED-4DA8-A615-8AFFD9E1BC6C}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B22:B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2463,7 +2463,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2479,7 +2479,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,7 +2487,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2495,7 +2495,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2503,7 +2503,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2511,7 +2511,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2519,7 +2519,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2527,7 +2527,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>200000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2551,7 +2551,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,7 +2575,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2583,7 +2583,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2591,7 +2591,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2599,7 +2599,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2615,7 +2615,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2623,7 +2623,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2631,7 +2631,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2647,7 +2647,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2655,7 +2655,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2663,7 +2663,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,7 +2679,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2687,7 +2687,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2703,7 +2703,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2711,7 +2711,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2719,7 +2719,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2727,7 +2727,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2735,7 +2735,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2759,7 +2759,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2767,7 +2767,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>-2000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2775,7 +2775,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2783,7 +2783,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2799,7 +2799,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2807,7 +2807,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2815,7 +2815,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2823,7 +2823,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2831,7 +2831,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2839,7 +2839,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2847,7 +2847,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added islanding transition logic and updated grid connected battery hi/low SOC logic. Dealt with some wind oscillation/startup issues, sometimes still have issues.
</commit_message>
<xml_diff>
--- a/CART dependencies/Microgrid_cmd.xlsx
+++ b/CART dependencies/Microgrid_cmd.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Autonomous-Microgrid-Control-with-Forecasting\CART dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8338241-CC3A-4974-88A1-2B8796ECC501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7B6038-A790-4C99-B13E-BB500D0AAF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
   </bookViews>
   <sheets>
     <sheet name="P_req" sheetId="13" r:id="rId1"/>
     <sheet name="Q_req" sheetId="15" r:id="rId2"/>
+    <sheet name="try_island" sheetId="16" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Time [s]</t>
   </si>
   <si>
     <t>mode</t>
+  </si>
+  <si>
+    <t>try_island</t>
   </si>
 </sst>
 </file>
@@ -398,7 +402,7 @@
   <dimension ref="A1:B452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B32"/>
+      <selection activeCell="B11" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +420,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>-1500000</v>
+        <v>-2000000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -424,7 +428,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>-1500000</v>
+        <v>-2000000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -432,7 +436,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>-1500000</v>
+        <v>-2000000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -440,7 +444,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>-1500000</v>
+        <v>-2000000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -448,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>-1500000</v>
+        <v>-2000000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -456,7 +460,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>-1500000</v>
+        <v>-2000000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +468,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -472,7 +476,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -480,7 +484,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -488,7 +492,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -496,7 +500,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -504,7 +508,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -512,7 +516,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,7 +524,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,7 +532,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,7 +540,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -544,7 +548,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -552,7 +556,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -560,7 +564,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -568,7 +572,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -576,7 +580,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -584,7 +588,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -592,7 +596,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -600,7 +604,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -608,7 +612,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -616,7 +620,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -624,7 +628,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -632,7 +636,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -640,7 +644,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -648,7 +652,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -656,7 +660,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -664,7 +668,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -672,7 +676,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -680,7 +684,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -688,7 +692,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -696,7 +700,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -704,7 +708,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -712,7 +716,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -720,7 +724,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -728,7 +732,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -736,7 +740,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -744,7 +748,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -752,7 +756,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -760,7 +764,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,7 +772,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -776,7 +780,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,7 +788,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -792,7 +796,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,7 +804,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +812,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -816,7 +820,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2429,7 +2433,7 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B32"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2455,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2463,7 +2467,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,7 +2475,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2479,7 +2483,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,7 +2491,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2495,7 +2499,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2503,7 +2507,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2511,7 +2515,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2519,7 +2523,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2527,7 +2531,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>-1500000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2535,7 +2539,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2543,7 +2547,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2551,7 +2555,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2559,7 +2563,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2567,7 +2571,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,7 +2579,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2583,7 +2587,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2591,7 +2595,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2599,7 +2603,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2607,7 +2611,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2615,7 +2619,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2623,7 +2627,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2631,7 +2635,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2639,7 +2643,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2647,7 +2651,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2655,7 +2659,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2663,7 +2667,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2671,7 +2675,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,7 +2683,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2687,7 +2691,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2695,7 +2699,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2703,7 +2707,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2711,7 +2715,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2719,7 +2723,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2727,7 +2731,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2735,7 +2739,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2743,7 +2747,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2751,7 +2755,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2759,7 +2763,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2767,7 +2771,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2775,7 +2779,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2783,7 +2787,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2791,7 +2795,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2799,7 +2803,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2807,7 +2811,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2815,7 +2819,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2823,7 +2827,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2831,7 +2835,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2839,7 +2843,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3">
-        <v>200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2847,7 +2851,438 @@
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>200000</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2541F847-412C-4CAF-A52B-A1D85C823AC7}">
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated MGCC so that BESS is in grid following mode when grid connected and seeks target SOC. First draft of MGCC done
</commit_message>
<xml_diff>
--- a/CART dependencies/Microgrid_cmd.xlsx
+++ b/CART dependencies/Microgrid_cmd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Autonomous-Microgrid-Control-with-Forecasting\CART dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7B6038-A790-4C99-B13E-BB500D0AAF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70BF828-313D-4FDF-A490-E680A8F13CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
   </bookViews>
   <sheets>
     <sheet name="P_req" sheetId="13" r:id="rId1"/>
@@ -401,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43E032D-C64D-4416-8490-73EE1F87088C}">
   <dimension ref="A1:B452"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B8:B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +420,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>-2000000</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -428,7 +428,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>-2000000</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -436,7 +436,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>-2000000</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -444,7 +444,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>-2000000</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>-2000000</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -460,7 +460,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>-2000000</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,7 +468,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,7 +484,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -492,7 +492,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -500,7 +500,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2863,8 +2863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2541F847-412C-4CAF-A52B-A1D85C823AC7}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3018,7 +3018,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3034,7 +3034,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3042,7 +3042,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3050,7 +3050,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3058,7 +3058,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3066,7 +3066,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3074,7 +3074,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3082,7 +3082,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3090,7 +3090,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3098,7 +3098,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -3106,7 +3106,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3114,7 +3114,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3122,7 +3122,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3130,7 +3130,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3138,7 +3138,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3146,7 +3146,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3154,7 +3154,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added PV disconnect to prevent it tanking the MG during faults
</commit_message>
<xml_diff>
--- a/CART dependencies/Microgrid_cmd.xlsx
+++ b/CART dependencies/Microgrid_cmd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Autonomous-Microgrid-Control-with-Forecasting\CART dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70BF828-313D-4FDF-A490-E680A8F13CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0105837A-702F-42BA-9FF5-AE119612468F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
   </bookViews>
@@ -401,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43E032D-C64D-4416-8490-73EE1F87088C}">
   <dimension ref="A1:B452"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B38"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +420,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -428,7 +428,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -436,7 +436,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -444,7 +444,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -460,7 +460,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,7 +468,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,7 +484,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -492,7 +492,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -500,7 +500,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>-1400000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>-1400000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -820,7 +820,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>0</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2425,6 +2425,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2433,7 +2434,7 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2861,10 +2862,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2541F847-412C-4CAF-A52B-A1D85C823AC7}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B18"/>
+      <selection activeCell="F5" sqref="E4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2882,7 +2883,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2890,7 +2891,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3018,7 +3019,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3026,7 +3027,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3034,7 +3035,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3042,7 +3043,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3050,7 +3051,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3058,7 +3059,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3066,7 +3067,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3074,7 +3075,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3082,7 +3083,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3090,7 +3091,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3098,7 +3099,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -3106,7 +3107,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3114,7 +3115,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3122,7 +3123,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3130,7 +3131,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3138,7 +3139,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3146,7 +3147,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3154,7 +3155,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3162,7 +3163,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3178,7 +3179,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3186,7 +3187,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3194,7 +3195,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3202,7 +3203,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3210,7 +3211,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3218,7 +3219,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3226,7 +3227,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3234,7 +3235,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3242,7 +3243,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3250,7 +3251,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3258,7 +3259,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3266,7 +3267,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3274,7 +3275,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3282,7 +3283,87 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added forecasting/targetSOC logic. Next will update WT modes as a vector for [P, Q]
</commit_message>
<xml_diff>
--- a/CART dependencies/Microgrid_cmd.xlsx
+++ b/CART dependencies/Microgrid_cmd.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Autonomous-Microgrid-Control-with-Forecasting\CART dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0105837A-702F-42BA-9FF5-AE119612468F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733E85A6-3424-4CFF-B8BD-61A44D536BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
   </bookViews>
@@ -2865,7 +2865,7 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="E4:F5"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2883,7 +2883,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2899,7 +2899,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2907,7 +2907,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>